<commit_message>
agregamos KIIA y actualizamos Anahuac
</commit_message>
<xml_diff>
--- a/AnahuacPuebla/assets/excel/talleres.xlsx
+++ b/AnahuacPuebla/assets/excel/talleres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\yellowhat\proyectos\yellowhatonline.demo\AnahuacPuebla\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B5212A-85E6-4625-9118-931A723F7AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA784105-4001-4EA4-81A7-4C207561E041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{7A8DAA02-A1C6-4A03-8B94-E2D69863ED3B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -255,13 +255,16 @@
   </si>
   <si>
     <t>Turismo Internacional</t>
+  </si>
+  <si>
+    <t>Nombre Licenciatura</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +278,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -297,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -305,12 +316,168 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13.5"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -321,6 +488,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B34E139D-E02A-4233-AB65-EB5511CE54B6}" name="Tabla1" displayName="Tabla1" ref="A1:B44" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:B44" xr:uid="{B34E139D-E02A-4233-AB65-EB5511CE54B6}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2D8D8B1D-5185-430A-81D4-3D35AF582DBA}" name="ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3D7D1725-CC78-4B81-92E8-D4DE00ABA0B6}" name="Nombre" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{995A0C86-2F27-48AE-98B5-EC3A3DB40A86}" name="Tabla2" displayName="Tabla2" ref="A1:B44" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:B44" xr:uid="{995A0C86-2F27-48AE-98B5-EC3A3DB40A86}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FCF1BB5A-4149-452A-B410-F9B4D33DE98A}" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D9F5ADFD-0B4A-4A65-8AAE-A1513E1349D5}" name="Nombre" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{678D71ED-84DE-47E2-B889-88868BA5C354}" name="Tabla3" displayName="Tabla3" ref="A1:B43" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:B43" xr:uid="{678D71ED-84DE-47E2-B889-88868BA5C354}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{45490B96-2C3F-4CEE-9D38-EA1D8FB2B723}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{0A20CEDF-66B2-4EE4-A26F-A753FA1E818B}" name="Nombre" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D17AC786-54B0-4FE7-A0B4-14EFAF740BF3}" name="Tabla4" displayName="Tabla4" ref="A1:B26" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B26" xr:uid="{D17AC786-54B0-4FE7-A0B4-14EFAF740BF3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{DCC28433-5A7A-4305-B658-86D670ABA2C0}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3D849F15-8E85-495C-9226-386F9CCE7D3D}" name="Nombre Licenciatura" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -620,543 +831,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE3859A-9036-4E42-A4CE-05758C4E1F60}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B44"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="3"/>
     <col min="2" max="2" width="116.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <f>LEN(B2)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C44" si="0">LEN(B3)</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5">
+    </row>
+    <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6">
+    </row>
+    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7">
+    </row>
+    <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8">
+    </row>
+    <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9">
+    </row>
+    <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10">
+    </row>
+    <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11">
+    </row>
+    <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12">
+    </row>
+    <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13">
+    </row>
+    <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14">
+    </row>
+    <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15">
+    </row>
+    <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16">
+    </row>
+    <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17">
+    </row>
+    <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18">
+    </row>
+    <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19">
+    </row>
+    <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20">
+    </row>
+    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A21">
+    </row>
+    <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22">
+    </row>
+    <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23">
+    </row>
+    <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24">
+    </row>
+    <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25">
+    </row>
+    <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26">
+    </row>
+    <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A27">
+    </row>
+    <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28">
+    </row>
+    <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A29">
+    </row>
+    <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30">
+    </row>
+    <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A31">
+    </row>
+    <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A32">
+    </row>
+    <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A33">
+    </row>
+    <row r="33" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A34">
+    </row>
+    <row r="34" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A35">
+    </row>
+    <row r="35" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36">
+    </row>
+    <row r="36" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C36">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A37">
+    </row>
+    <row r="37" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A38">
+    </row>
+    <row r="38" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39">
+    </row>
+    <row r="39" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C39">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A40">
+    </row>
+    <row r="40" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C40">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41">
+    </row>
+    <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C41">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A42">
+    </row>
+    <row r="42" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C42">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A43">
+    </row>
+    <row r="43" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C43">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A44">
+    </row>
+    <row r="44" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C44">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1164,25 +1207,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F5EF3C-F091-4BD6-BA42-079AF9F28899}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B44"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="3"/>
     <col min="2" max="2" width="116.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1190,7 +1234,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1198,7 +1242,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1206,7 +1250,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1214,7 +1258,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1222,7 +1266,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1230,7 +1274,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1238,7 +1282,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1246,7 +1290,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1254,7 +1298,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1262,7 +1306,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1270,7 +1314,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1278,7 +1322,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1286,7 +1330,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1294,7 +1338,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1302,7 +1346,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1310,7 +1354,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1318,7 +1362,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1326,7 +1370,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1334,7 +1378,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1342,7 +1386,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1350,7 +1394,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1358,7 +1402,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1366,7 +1410,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1374,7 +1418,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1382,7 +1426,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1390,7 +1434,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1398,7 +1442,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1406,7 +1450,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1414,7 +1458,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1422,7 +1466,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1430,7 +1474,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1438,7 +1482,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1446,7 +1490,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1454,7 +1498,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1462,7 +1506,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1470,7 +1514,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1478,7 +1522,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1486,7 +1530,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1494,7 +1538,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1502,7 +1546,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1510,7 +1554,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1518,7 +1562,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1527,6 +1571,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1534,25 +1581,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28B146D-F93B-4193-85FD-FCB3C6E761E8}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B43"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="3"/>
     <col min="2" max="2" width="116.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1560,7 +1608,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1568,7 +1616,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1576,7 +1624,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1584,7 +1632,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1592,7 +1640,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1600,7 +1648,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1608,7 +1656,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1616,7 +1664,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1624,7 +1672,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1632,7 +1680,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1640,7 +1688,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1648,7 +1696,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1656,7 +1704,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1664,7 +1712,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1672,7 +1720,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1680,7 +1728,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1688,7 +1736,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1696,7 +1744,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1704,7 +1752,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1712,7 +1760,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1720,7 +1768,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1728,7 +1776,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1736,7 +1784,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1744,7 +1792,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1752,7 +1800,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1760,7 +1808,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1768,7 +1816,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1776,7 +1824,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1784,7 +1832,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1792,7 +1840,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1800,7 +1848,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1808,7 +1856,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1816,7 +1864,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1824,7 +1872,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1832,7 +1880,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1840,7 +1888,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1848,7 +1896,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1856,7 +1904,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1864,7 +1912,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1872,7 +1920,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1880,7 +1928,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1889,6 +1937,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1897,24 +1948,25 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B26"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
+      <c r="B1" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1922,7 +1974,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1930,7 +1982,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1938,7 +1990,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1946,7 +1998,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1954,7 +2006,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1962,7 +2014,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1970,7 +2022,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1978,7 +2030,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1986,7 +2038,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1994,7 +2046,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2002,7 +2054,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2010,7 +2062,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2018,7 +2070,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2026,7 +2078,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2034,7 +2086,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2042,7 +2094,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2050,7 +2102,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2058,7 +2110,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2066,7 +2118,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2074,7 +2126,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2082,7 +2134,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2090,7 +2142,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2098,7 +2150,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2106,7 +2158,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2115,5 +2167,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>